<commit_message>
update with suggestions from Leander
</commit_message>
<xml_diff>
--- a/geochemistry/AnalyticalMethodNotation.xlsx
+++ b/geochemistry/AnalyticalMethodNotation.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944a82e2ddcde9eb/Documents/GithubC/Astromat/Vocabulary/geochemistry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{DC6A8E47-B5AA-4822-9869-B2DEB139BBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="20" documentId="13_ncr:40009_{DC6A8E47-B5AA-4822-9869-B2DEB139BBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{473734D3-5FCA-4EE8-AC83-12DC82A04B0C}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="3180" yWindow="435" windowWidth="24675" windowHeight="16035" activeTab="1"/>
+    <workbookView xWindow="3525" yWindow="780" windowWidth="24675" windowHeight="16035" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalyticalMethodNotation" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Stephen Richard</author>
   </authors>
   <commentList>
-    <comment ref="D1" authorId="0" shapeId="0">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -37,7 +37,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>Stephen Richard:</t>
         </r>
@@ -46,7 +46,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 formula:   =VLOOKUP(C2,analyticalMethodSources.txt!$B$2:$C$246,2,FALSE)</t>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1333" uniqueCount="810">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="816">
   <si>
     <t>notation</t>
   </si>
@@ -2044,9 +2044,6 @@
   </si>
   <si>
     <t>https://unacademy.com/content/nta-ugc/study-material/pharmaceutical-analysis/polarography/ | https://w3id.org/geochem/1.0/agent/georoc | https://w3id.org/geochem/1.0/analyticalmethod/skooghollercrouch | https://en.wikipedia.org/wiki/Polarography</t>
-  </si>
-  <si>
-    <t>https://en.wikipedia.org/wiki/Porosimetry | https://w3id.org/geochem/1.0/analyticalmethod/smraddinstmethodsgeox</t>
   </si>
   <si>
     <t>https://doi.org/10.1515/pac-2018-0109 | https://w3id.org/geochem/1.0/agent/petdb | https://w3id.org/geochem/1.0/agent/astromat | https://w3id.org/geochem/1.0/agent/georoc | https://w3id.org/geochem/1.0/agent/geox</t>
@@ -2278,21 +2275,6 @@
       </rPr>
       <t xml:space="preserve"> 
 | https://doi.org/10.1515/pac-2018-0109</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">https://www.xos.com/Confocal-XRF | </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>https://w3id.org/geochem/1.0/agent/orex</t>
     </r>
   </si>
   <si>
@@ -2717,9 +2699,6 @@
     </r>
   </si>
   <si>
-    <t>GeoRoc uses IQ for "INFRARED QUANTIFICATION AND HIGH TEMPERATURE EVOLUTION ANALYSIS" that is an alt label for this method</t>
-  </si>
-  <si>
     <t>EDS-M</t>
   </si>
   <si>
@@ -2806,12 +2785,76 @@
   </si>
   <si>
     <t xml:space="preserve">yellow boxes are methods, mostly from Geo.X or GeoRoc, that need notations.  </t>
+  </si>
+  <si>
+    <t>DTA</t>
+  </si>
+  <si>
+    <t>suggested by Leander</t>
+  </si>
+  <si>
+    <t>EA-IR</t>
+  </si>
+  <si>
+    <t>GeoRoc uses IQ for "INFRARED QUANTIFICATION AND HIGH TEMPERATURE EVOLUTION ANALYSIS" that is an alt label for this method; Leander suggested EAIR, SMR modified to EA-IR for consistency with other EA- methods.  I was interpreting Elemental Analysis to be the same thing as High-Temperature Evolution....</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PIGCNAA </t>
+  </si>
+  <si>
+    <t>suggested by Leander/GeoRoc.</t>
+  </si>
+  <si>
+    <r>
+      <t>https://en.wikipedia.org/wiki/Porosimetry | https://w3id.org/geochem/1.0/analyticalmethod/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>smraddinstmethodsgeox</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>https://w3id.org/geochem/1.0/analyticalmethod/</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>smraddinstmethodsgeox</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">https://www.xos.com/Confocal-XRF 
+| </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>https://w3id.org/geochem/1.0/agent/orex</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2951,14 +2994,14 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -3335,7 +3378,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3349,27 +3392,17 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="2" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="33" borderId="1" xfId="2" applyFill="1" applyAlignment="1">
@@ -3387,6 +3420,7 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3767,12 +3801,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G246"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A46" sqref="A46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3839,7 +3873,7 @@
         <v>10</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>693</v>
+        <v>692</v>
       </c>
       <c r="E3" s="3"/>
       <c r="F3" s="2" t="s">
@@ -3850,7 +3884,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="7" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -3859,7 +3893,7 @@
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" t="s">
         <v>586</v>
       </c>
       <c r="E4" s="3" t="s">
@@ -3900,7 +3934,7 @@
         <v>21</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>692</v>
+        <v>691</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="2" t="s">
@@ -3919,7 +3953,7 @@
         <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="2" t="s">
@@ -3978,7 +4012,7 @@
         <v>30</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>694</v>
+        <v>693</v>
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2" t="s">
@@ -3997,7 +4031,7 @@
         <v>32</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>719</v>
+        <v>718</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>33</v>
@@ -4008,7 +4042,7 @@
       <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2" t="s">
         <v>34</v>
@@ -4107,10 +4141,10 @@
         <v>43</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>774</v>
+        <v>772</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>772</v>
+        <v>770</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>22</v>
@@ -4177,7 +4211,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="8"/>
+      <c r="A21" s="7"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2" t="s">
         <v>53</v>
@@ -4198,7 +4232,7 @@
         <v>54</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="2" t="s">
@@ -4209,7 +4243,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="8"/>
+      <c r="A23" s="7"/>
       <c r="B23" s="2"/>
       <c r="C23" s="2" t="s">
         <v>56</v>
@@ -4420,13 +4454,13 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="8"/>
+      <c r="A34" s="7"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2" t="s">
         <v>85</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>776</v>
+        <v>774</v>
       </c>
       <c r="E34" s="3"/>
       <c r="F34" s="2"/>
@@ -4483,7 +4517,7 @@
         <v>94</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
       <c r="E37" s="3"/>
       <c r="F37" s="2" t="s">
@@ -4512,22 +4546,22 @@
         <v>93</v>
       </c>
     </row>
-    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>97</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>720</v>
+        <v>815</v>
       </c>
       <c r="E39" s="3" t="s">
+        <v>773</v>
+      </c>
+      <c r="F39" s="2" t="s">
         <v>775</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>777</v>
       </c>
       <c r="G39" s="2"/>
     </row>
@@ -4639,7 +4673,7 @@
         <v>110</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>697</v>
+        <v>696</v>
       </c>
       <c r="E45" s="3"/>
       <c r="F45" s="2" t="s">
@@ -4650,15 +4684,19 @@
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="16"/>
-      <c r="B46" s="2"/>
+      <c r="A46" s="12"/>
+      <c r="B46" s="2" t="s">
+        <v>807</v>
+      </c>
       <c r="C46" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="D46" s="6" t="s">
+      <c r="D46" s="5" t="s">
         <v>598</v>
       </c>
-      <c r="E46" s="3"/>
+      <c r="E46" s="3" t="s">
+        <v>808</v>
+      </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2"/>
     </row>
@@ -4714,7 +4752,7 @@
       <c r="C49" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="D49" s="4" t="s">
+      <c r="D49" s="15" t="s">
         <v>585</v>
       </c>
       <c r="E49" s="3"/>
@@ -4726,13 +4764,13 @@
       </c>
     </row>
     <row r="50" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="16"/>
+      <c r="A50" s="12"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2" t="s">
         <v>121</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="E50" s="3"/>
       <c r="F50" s="2"/>
@@ -4760,7 +4798,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="16"/>
+      <c r="A52" s="12"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2" t="s">
         <v>125</v>
@@ -4769,7 +4807,7 @@
         <v>612</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="F52" s="2"/>
       <c r="G52" s="2"/>
@@ -4836,12 +4874,12 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="8"/>
+      <c r="A56" s="7"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" t="s">
         <v>595</v>
       </c>
       <c r="E56" s="3"/>
@@ -4851,19 +4889,19 @@
     <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
       <c r="B57" s="2" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C57" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="D57" s="10" t="s">
-        <v>780</v>
+      <c r="D57" s="3" t="s">
+        <v>778</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="G57" s="2"/>
     </row>
@@ -4991,17 +5029,19 @@
         <v>105</v>
       </c>
     </row>
-    <row r="64" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A64" s="16"/>
-      <c r="B64" s="2"/>
+    <row r="64" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+      <c r="A64" s="12"/>
+      <c r="B64" s="2" t="s">
+        <v>809</v>
+      </c>
       <c r="C64" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D64" s="12" t="s">
+      <c r="D64" s="8" t="s">
         <v>598</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>781</v>
+        <v>810</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2"/>
@@ -5017,7 +5057,7 @@
         <v>161</v>
       </c>
       <c r="D65" s="3" t="s">
-        <v>698</v>
+        <v>697</v>
       </c>
       <c r="E65" s="3"/>
       <c r="F65" s="2" t="s">
@@ -5101,7 +5141,7 @@
         <v>174</v>
       </c>
       <c r="D69" s="3" t="s">
-        <v>699</v>
+        <v>698</v>
       </c>
       <c r="E69" s="3"/>
       <c r="F69" s="2" t="s">
@@ -5111,22 +5151,22 @@
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
       <c r="B70" s="2" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="C70" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="D70" s="13" t="s">
+      <c r="D70" s="9" t="s">
         <v>585</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>783</v>
+        <v>780</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>782</v>
+        <v>779</v>
       </c>
       <c r="G70" s="2"/>
     </row>
@@ -5259,7 +5299,7 @@
         <v>193</v>
       </c>
       <c r="D77" s="3" t="s">
-        <v>700</v>
+        <v>699</v>
       </c>
       <c r="E77" s="3"/>
       <c r="F77" s="2" t="s">
@@ -5291,26 +5331,26 @@
       </c>
     </row>
     <row r="79" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A79" s="16"/>
+      <c r="A79" s="12"/>
       <c r="B79" s="2"/>
       <c r="C79" s="2" t="s">
         <v>198</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>722</v>
+        <v>720</v>
       </c>
       <c r="E79" s="3"/>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
     </row>
     <row r="80" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A80" s="16"/>
+      <c r="A80" s="12"/>
       <c r="B80" s="2"/>
       <c r="C80" s="2" t="s">
         <v>199</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>723</v>
+        <v>721</v>
       </c>
       <c r="E80" s="3"/>
       <c r="F80" s="2"/>
@@ -5415,7 +5455,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="86" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>211</v>
       </c>
@@ -5508,7 +5548,7 @@
         <v>222</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="E90" s="3"/>
       <c r="F90" s="2" t="s">
@@ -5557,7 +5597,7 @@
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A93" s="8"/>
+      <c r="A93" s="7"/>
       <c r="B93" s="2"/>
       <c r="C93" s="2" t="s">
         <v>228</v>
@@ -5669,20 +5709,20 @@
       </c>
     </row>
     <row r="99" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A99" s="16"/>
+      <c r="A99" s="12"/>
       <c r="B99" s="2"/>
       <c r="C99" s="2" t="s">
         <v>238</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>724</v>
+        <v>722</v>
       </c>
       <c r="E99" s="3"/>
       <c r="F99" s="2"/>
       <c r="G99" s="2"/>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="8"/>
+      <c r="A100" s="7"/>
       <c r="B100" s="2"/>
       <c r="C100" s="2" t="s">
         <v>239</v>
@@ -5798,7 +5838,7 @@
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A106" s="8"/>
+      <c r="A106" s="7"/>
       <c r="B106" s="2"/>
       <c r="C106" s="2" t="s">
         <v>255</v>
@@ -5859,7 +5899,7 @@
         <v>263</v>
       </c>
       <c r="D109" s="3" t="s">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="E109" s="3"/>
       <c r="F109" s="2" t="s">
@@ -5899,7 +5939,7 @@
         <v>269</v>
       </c>
       <c r="D111" s="3" t="s">
-        <v>703</v>
+        <v>702</v>
       </c>
       <c r="E111" s="3"/>
       <c r="F111" s="2" t="s">
@@ -5918,7 +5958,7 @@
         <v>270</v>
       </c>
       <c r="D112" s="3" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="E112" s="3"/>
       <c r="F112" s="2" t="s">
@@ -6021,7 +6061,7 @@
         <v>285</v>
       </c>
       <c r="D117" s="3" t="s">
-        <v>705</v>
+        <v>704</v>
       </c>
       <c r="E117" s="3"/>
       <c r="F117" s="2" t="s">
@@ -6063,7 +6103,7 @@
         <v>292</v>
       </c>
       <c r="D119" s="3" t="s">
-        <v>706</v>
+        <v>705</v>
       </c>
       <c r="E119" s="3"/>
       <c r="F119" s="2" t="s">
@@ -6084,7 +6124,7 @@
         <v>295</v>
       </c>
       <c r="D120" s="3" t="s">
-        <v>707</v>
+        <v>706</v>
       </c>
       <c r="E120" s="3"/>
       <c r="F120" s="2" t="s">
@@ -6238,19 +6278,19 @@
     <row r="128" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
       <c r="B128" s="2" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="C128" s="2" t="s">
         <v>315</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>725</v>
+        <v>723</v>
       </c>
       <c r="E128" s="3" t="s">
-        <v>785</v>
+        <v>782</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>784</v>
+        <v>781</v>
       </c>
       <c r="G128" s="2"/>
     </row>
@@ -6274,16 +6314,16 @@
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="16"/>
+      <c r="A130" s="12"/>
       <c r="B130" s="2"/>
       <c r="C130" s="2" t="s">
         <v>317</v>
       </c>
       <c r="D130" s="3" t="s">
-        <v>612</v>
+        <v>814</v>
       </c>
       <c r="E130" s="3" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="F130" s="2"/>
       <c r="G130" s="2"/>
@@ -6318,7 +6358,7 @@
         <v>321</v>
       </c>
       <c r="D132" s="3" t="s">
-        <v>708</v>
+        <v>707</v>
       </c>
       <c r="E132" s="3"/>
       <c r="F132" s="2" t="s">
@@ -6411,16 +6451,16 @@
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" s="16"/>
+      <c r="A137" s="12"/>
       <c r="B137" s="2"/>
       <c r="C137" s="2" t="s">
         <v>335</v>
       </c>
       <c r="D137" s="3" t="s">
-        <v>612</v>
+        <v>814</v>
       </c>
       <c r="E137" s="3" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="F137" s="2"/>
       <c r="G137" s="2"/>
@@ -6484,7 +6524,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="141" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A141" s="2" t="s">
         <v>344</v>
       </c>
@@ -6507,7 +6547,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="142" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A142" s="2" t="s">
         <v>347</v>
       </c>
@@ -6521,7 +6561,7 @@
         <v>585</v>
       </c>
       <c r="E142" s="3" t="s">
-        <v>773</v>
+        <v>771</v>
       </c>
       <c r="F142" s="2" t="s">
         <v>348</v>
@@ -6581,7 +6621,7 @@
         <v>358</v>
       </c>
       <c r="D145" s="3" t="s">
-        <v>709</v>
+        <v>708</v>
       </c>
       <c r="E145" s="3"/>
       <c r="F145" s="2" t="s">
@@ -6793,27 +6833,27 @@
         <v>357</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A156" s="2"/>
       <c r="B156" s="2" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="C156" s="2" t="s">
         <v>384</v>
       </c>
       <c r="D156" s="3" t="s">
-        <v>726</v>
+        <v>724</v>
       </c>
       <c r="E156" s="3" t="s">
-        <v>786</v>
+        <v>783</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>787</v>
+        <v>784</v>
       </c>
       <c r="G156" s="2"/>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A157" s="8" t="s">
+      <c r="A157" s="7" t="s">
         <v>385</v>
       </c>
       <c r="B157" s="2"/>
@@ -6832,7 +6872,7 @@
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A158" s="8" t="s">
+      <c r="A158" s="7" t="s">
         <v>387</v>
       </c>
       <c r="B158" s="2" t="s">
@@ -6973,16 +7013,16 @@
       </c>
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A165" s="16"/>
+      <c r="A165" s="12"/>
       <c r="B165" s="2"/>
       <c r="C165" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="D165" s="3" t="s">
-        <v>612</v>
+      <c r="D165" s="15" t="s">
+        <v>814</v>
       </c>
       <c r="E165" s="3" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="F165" s="2"/>
       <c r="G165" s="2"/>
@@ -7047,7 +7087,7 @@
       </c>
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A169" s="8"/>
+      <c r="A169" s="7"/>
       <c r="B169" s="2"/>
       <c r="C169" s="2" t="s">
         <v>415</v>
@@ -7188,16 +7228,16 @@
       </c>
     </row>
     <row r="176" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A176" s="16"/>
+      <c r="A176" s="12"/>
       <c r="B176" s="2"/>
       <c r="C176" s="2" t="s">
         <v>435</v>
       </c>
       <c r="D176" s="3" t="s">
-        <v>662</v>
+        <v>813</v>
       </c>
       <c r="E176" s="3" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="F176" s="2"/>
       <c r="G176" s="2"/>
@@ -7232,7 +7272,7 @@
         <v>439</v>
       </c>
       <c r="D178" s="3" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
       <c r="E178" s="3"/>
       <c r="F178" s="2" t="s">
@@ -7243,15 +7283,19 @@
       </c>
     </row>
     <row r="179" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A179" s="16"/>
-      <c r="B179" s="2"/>
+      <c r="A179" s="12"/>
+      <c r="B179" s="2" t="s">
+        <v>811</v>
+      </c>
       <c r="C179" s="2" t="s">
         <v>440</v>
       </c>
       <c r="D179" s="3" t="s">
-        <v>727</v>
-      </c>
-      <c r="E179" s="3"/>
+        <v>725</v>
+      </c>
+      <c r="E179" s="3" t="s">
+        <v>812</v>
+      </c>
       <c r="F179" s="2"/>
       <c r="G179" s="2"/>
     </row>
@@ -7264,7 +7308,7 @@
         <v>442</v>
       </c>
       <c r="D180" s="3" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
       <c r="E180" s="3"/>
       <c r="F180" s="2" t="s">
@@ -7285,7 +7329,7 @@
         <v>444</v>
       </c>
       <c r="D181" s="3" t="s">
-        <v>711</v>
+        <v>710</v>
       </c>
       <c r="E181" s="3"/>
       <c r="F181" s="2" t="s">
@@ -7327,7 +7371,7 @@
         <v>449</v>
       </c>
       <c r="D183" s="3" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
       <c r="E183" s="3"/>
       <c r="F183" s="2" t="s">
@@ -7358,7 +7402,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="185" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
         <v>452</v>
       </c>
@@ -7369,7 +7413,7 @@
         <v>454</v>
       </c>
       <c r="D185" s="3" t="s">
-        <v>666</v>
+        <v>665</v>
       </c>
       <c r="E185" s="3" t="s">
         <v>455</v>
@@ -7392,7 +7436,7 @@
         <v>458</v>
       </c>
       <c r="D186" s="3" t="s">
-        <v>667</v>
+        <v>666</v>
       </c>
       <c r="E186" s="3" t="s">
         <v>459</v>
@@ -7415,7 +7459,7 @@
         <v>462</v>
       </c>
       <c r="D187" s="3" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
       <c r="E187" s="3"/>
       <c r="F187" s="2" t="s">
@@ -7453,7 +7497,7 @@
         <v>467</v>
       </c>
       <c r="D189" s="3" t="s">
-        <v>669</v>
+        <v>668</v>
       </c>
       <c r="E189" s="3"/>
       <c r="F189" s="2" t="s">
@@ -7474,7 +7518,7 @@
         <v>470</v>
       </c>
       <c r="D190" s="3" t="s">
-        <v>710</v>
+        <v>709</v>
       </c>
       <c r="E190" s="3"/>
       <c r="F190" s="2" t="s">
@@ -7485,13 +7529,13 @@
       </c>
     </row>
     <row r="191" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A191" s="16"/>
+      <c r="A191" s="12"/>
       <c r="B191" s="2"/>
       <c r="C191" s="2" t="s">
         <v>471</v>
       </c>
       <c r="D191" s="3" t="s">
-        <v>728</v>
+        <v>726</v>
       </c>
       <c r="E191" s="3"/>
       <c r="F191" s="2"/>
@@ -7500,19 +7544,19 @@
     <row r="192" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A192" s="2"/>
       <c r="B192" s="2" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="C192" s="2" t="s">
         <v>472</v>
       </c>
-      <c r="D192" s="15" t="s">
-        <v>793</v>
+      <c r="D192" s="11" t="s">
+        <v>790</v>
       </c>
       <c r="E192" s="3" t="s">
-        <v>792</v>
+        <v>789</v>
       </c>
       <c r="F192" s="2" t="s">
-        <v>791</v>
+        <v>788</v>
       </c>
       <c r="G192" s="2"/>
     </row>
@@ -7538,13 +7582,13 @@
       </c>
     </row>
     <row r="194" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A194" s="16"/>
+      <c r="A194" s="12"/>
       <c r="B194" s="2"/>
       <c r="C194" s="2" t="s">
         <v>476</v>
       </c>
       <c r="D194" s="3" t="s">
-        <v>729</v>
+        <v>727</v>
       </c>
       <c r="E194" s="3"/>
       <c r="F194" s="2"/>
@@ -7559,7 +7603,7 @@
         <v>478</v>
       </c>
       <c r="D195" s="3" t="s">
-        <v>670</v>
+        <v>669</v>
       </c>
       <c r="E195" s="3"/>
       <c r="F195" s="2" t="s">
@@ -7578,7 +7622,7 @@
         <v>479</v>
       </c>
       <c r="D196" s="3" t="s">
-        <v>712</v>
+        <v>711</v>
       </c>
       <c r="E196" s="3"/>
       <c r="F196" s="2" t="s">
@@ -7599,7 +7643,7 @@
         <v>482</v>
       </c>
       <c r="D197" s="3" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
       <c r="E197" s="3"/>
       <c r="F197" s="2" t="s">
@@ -7620,7 +7664,7 @@
         <v>485</v>
       </c>
       <c r="D198" s="3" t="s">
-        <v>672</v>
+        <v>671</v>
       </c>
       <c r="E198" s="3"/>
       <c r="F198" s="2" t="s">
@@ -7641,7 +7685,7 @@
         <v>488</v>
       </c>
       <c r="D199" s="3" t="s">
-        <v>673</v>
+        <v>672</v>
       </c>
       <c r="E199" s="3"/>
       <c r="F199" s="2" t="s">
@@ -7681,7 +7725,7 @@
         <v>493</v>
       </c>
       <c r="D201" s="3" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
       <c r="E201" s="3" t="s">
         <v>494</v>
@@ -7694,26 +7738,26 @@
       </c>
     </row>
     <row r="202" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A202" s="16"/>
+      <c r="A202" s="12"/>
       <c r="B202" s="2"/>
       <c r="C202" s="2" t="s">
         <v>495</v>
       </c>
       <c r="D202" s="3" t="s">
-        <v>721</v>
+        <v>719</v>
       </c>
       <c r="E202" s="3"/>
       <c r="F202" s="2"/>
       <c r="G202" s="2"/>
     </row>
     <row r="203" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A203" s="16"/>
+      <c r="A203" s="12"/>
       <c r="B203" s="2"/>
       <c r="C203" s="2" t="s">
         <v>496</v>
       </c>
       <c r="D203" s="3" t="s">
-        <v>730</v>
+        <v>728</v>
       </c>
       <c r="E203" s="3"/>
       <c r="F203" s="2"/>
@@ -7751,7 +7795,7 @@
         <v>502</v>
       </c>
       <c r="D205" s="3" t="s">
-        <v>713</v>
+        <v>712</v>
       </c>
       <c r="E205" s="3" t="s">
         <v>503</v>
@@ -7774,7 +7818,7 @@
         <v>506</v>
       </c>
       <c r="D206" s="3" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
       <c r="E206" s="3" t="s">
         <v>507</v>
@@ -7797,7 +7841,7 @@
         <v>511</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>714</v>
+        <v>713</v>
       </c>
       <c r="E207" s="3"/>
       <c r="F207" s="2" t="s">
@@ -7818,7 +7862,7 @@
         <v>514</v>
       </c>
       <c r="D208" s="3" t="s">
-        <v>676</v>
+        <v>675</v>
       </c>
       <c r="E208" s="3"/>
       <c r="F208" s="2" t="s">
@@ -7856,7 +7900,7 @@
         <v>517</v>
       </c>
       <c r="D210" s="3" t="s">
-        <v>677</v>
+        <v>676</v>
       </c>
       <c r="E210" s="3"/>
       <c r="F210" s="2" t="s">
@@ -7917,7 +7961,7 @@
         <v>526</v>
       </c>
       <c r="D213" s="3" t="s">
-        <v>678</v>
+        <v>677</v>
       </c>
       <c r="E213" s="3"/>
       <c r="F213" s="2" t="s">
@@ -7957,7 +8001,7 @@
         <v>529</v>
       </c>
       <c r="D215" s="3" t="s">
-        <v>679</v>
+        <v>678</v>
       </c>
       <c r="E215" s="3"/>
       <c r="F215" s="2" t="s">
@@ -7968,16 +8012,16 @@
       </c>
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A216" s="16"/>
+      <c r="A216" s="12"/>
       <c r="B216" s="2"/>
       <c r="C216" s="2" t="s">
         <v>530</v>
       </c>
-      <c r="D216" s="5" t="s">
+      <c r="D216" t="s">
         <v>612</v>
       </c>
       <c r="E216" s="3" t="s">
-        <v>788</v>
+        <v>785</v>
       </c>
       <c r="F216" s="2"/>
       <c r="G216" s="2"/>
@@ -8014,7 +8058,7 @@
         <v>536</v>
       </c>
       <c r="D218" s="3" t="s">
-        <v>680</v>
+        <v>679</v>
       </c>
       <c r="E218" s="3"/>
       <c r="F218" s="2" t="s">
@@ -8024,22 +8068,22 @@
         <v>515</v>
       </c>
     </row>
-    <row r="219" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A219" s="2"/>
       <c r="B219" s="2" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="C219" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="D219" s="9" t="s">
-        <v>805</v>
+      <c r="D219" s="1" t="s">
+        <v>802</v>
       </c>
       <c r="E219" s="3" t="s">
-        <v>795</v>
+        <v>792</v>
       </c>
       <c r="F219" s="2" t="s">
-        <v>794</v>
+        <v>791</v>
       </c>
       <c r="G219" s="2"/>
     </row>
@@ -8052,7 +8096,7 @@
         <v>538</v>
       </c>
       <c r="D220" s="3" t="s">
-        <v>681</v>
+        <v>680</v>
       </c>
       <c r="E220" s="3"/>
       <c r="F220" s="2" t="s">
@@ -8065,36 +8109,36 @@
     <row r="221" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
       <c r="B221" s="2" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="C221" s="2" t="s">
         <v>539</v>
       </c>
       <c r="D221" s="3" t="s">
-        <v>731</v>
+        <v>729</v>
       </c>
       <c r="E221" s="3" t="s">
-        <v>798</v>
+        <v>795</v>
       </c>
       <c r="F221" s="2" t="s">
-        <v>796</v>
+        <v>793</v>
       </c>
       <c r="G221" s="2"/>
     </row>
     <row r="222" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A222" s="2"/>
       <c r="B222" s="2" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="C222" s="2" t="s">
         <v>540</v>
       </c>
       <c r="D222" s="3" t="s">
-        <v>732</v>
+        <v>730</v>
       </c>
       <c r="E222" s="3"/>
       <c r="F222" s="2" t="s">
-        <v>797</v>
+        <v>794</v>
       </c>
       <c r="G222" s="2"/>
     </row>
@@ -8107,7 +8151,7 @@
         <v>542</v>
       </c>
       <c r="D223" s="3" t="s">
-        <v>682</v>
+        <v>681</v>
       </c>
       <c r="E223" s="3"/>
       <c r="F223" s="2" t="s">
@@ -8128,7 +8172,7 @@
         <v>544</v>
       </c>
       <c r="D224" s="3" t="s">
-        <v>715</v>
+        <v>714</v>
       </c>
       <c r="E224" s="3"/>
       <c r="F224" s="2" t="s">
@@ -8168,7 +8212,7 @@
         <v>549</v>
       </c>
       <c r="D226" s="3" t="s">
-        <v>683</v>
+        <v>682</v>
       </c>
       <c r="E226" s="3"/>
       <c r="F226" s="2" t="s">
@@ -8202,19 +8246,19 @@
     <row r="228" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A228" s="2"/>
       <c r="B228" s="2" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="C228" s="2" t="s">
         <v>553</v>
       </c>
       <c r="D228" s="3" t="s">
-        <v>733</v>
+        <v>731</v>
       </c>
       <c r="E228" s="3" t="s">
-        <v>799</v>
+        <v>796</v>
       </c>
       <c r="F228" s="2" t="s">
-        <v>800</v>
+        <v>797</v>
       </c>
       <c r="G228" s="2"/>
     </row>
@@ -8286,7 +8330,7 @@
         <v>558</v>
       </c>
       <c r="D232" s="3" t="s">
-        <v>684</v>
+        <v>683</v>
       </c>
       <c r="E232" s="3"/>
       <c r="F232" s="2" t="s">
@@ -8307,7 +8351,7 @@
         <v>560</v>
       </c>
       <c r="D233" s="3" t="s">
-        <v>685</v>
+        <v>684</v>
       </c>
       <c r="E233" s="3"/>
       <c r="F233" s="2" t="s">
@@ -8318,21 +8362,21 @@
       </c>
     </row>
     <row r="234" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A234" s="11"/>
+      <c r="A234" s="2"/>
       <c r="B234" s="2" t="s">
-        <v>804</v>
+        <v>801</v>
       </c>
       <c r="C234" s="2" t="s">
         <v>561</v>
       </c>
       <c r="D234" s="3" t="s">
+        <v>798</v>
+      </c>
+      <c r="E234" s="3" t="s">
+        <v>800</v>
+      </c>
+      <c r="F234" s="2" t="s">
         <v>801</v>
-      </c>
-      <c r="E234" s="3" t="s">
-        <v>803</v>
-      </c>
-      <c r="F234" s="2" t="s">
-        <v>804</v>
       </c>
       <c r="G234" s="2"/>
     </row>
@@ -8345,7 +8389,7 @@
         <v>562</v>
       </c>
       <c r="D235" s="3" t="s">
-        <v>686</v>
+        <v>685</v>
       </c>
       <c r="E235" s="3"/>
       <c r="F235" s="2" t="s">
@@ -8366,7 +8410,7 @@
         <v>564</v>
       </c>
       <c r="D236" s="3" t="s">
-        <v>687</v>
+        <v>686</v>
       </c>
       <c r="E236" s="3"/>
       <c r="F236" s="2" t="s">
@@ -8387,7 +8431,7 @@
         <v>566</v>
       </c>
       <c r="D237" s="3" t="s">
-        <v>688</v>
+        <v>687</v>
       </c>
       <c r="E237" s="3"/>
       <c r="F237" s="2" t="s">
@@ -8444,7 +8488,7 @@
         <v>569</v>
       </c>
       <c r="D240" s="3" t="s">
-        <v>689</v>
+        <v>688</v>
       </c>
       <c r="E240" s="3"/>
       <c r="F240" s="2" t="s">
@@ -8463,7 +8507,7 @@
         <v>571</v>
       </c>
       <c r="D241" s="3" t="s">
-        <v>716</v>
+        <v>715</v>
       </c>
       <c r="E241" s="3" t="s">
         <v>579</v>
@@ -8484,7 +8528,7 @@
         <v>572</v>
       </c>
       <c r="D242" s="3" t="s">
-        <v>690</v>
+        <v>689</v>
       </c>
       <c r="E242" s="3"/>
       <c r="F242" s="2" t="s">
@@ -8503,7 +8547,7 @@
         <v>573</v>
       </c>
       <c r="D243" s="3" t="s">
-        <v>717</v>
+        <v>716</v>
       </c>
       <c r="E243" s="3"/>
       <c r="F243" s="2" t="s">
@@ -8516,19 +8560,19 @@
     <row r="244" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A244" s="2"/>
       <c r="B244" s="2" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="C244" s="2" t="s">
         <v>574</v>
       </c>
       <c r="D244" s="3" t="s">
-        <v>806</v>
+        <v>803</v>
       </c>
       <c r="E244" s="3" t="s">
-        <v>808</v>
+        <v>805</v>
       </c>
       <c r="F244" s="2" t="s">
-        <v>807</v>
+        <v>804</v>
       </c>
       <c r="G244" s="2"/>
     </row>
@@ -8541,7 +8585,7 @@
         <v>575</v>
       </c>
       <c r="D245" s="3" t="s">
-        <v>718</v>
+        <v>717</v>
       </c>
       <c r="E245" s="3"/>
       <c r="F245" s="2" t="s">
@@ -8573,22 +8617,21 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="F1:F246"/>
+  <autoFilter ref="F1:F246" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <hyperlinks>
-    <hyperlink ref="E17" r:id="rId1"/>
-    <hyperlink ref="D13" r:id="rId2"/>
-    <hyperlink ref="D49" r:id="rId3"/>
+    <hyperlink ref="E17" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D13" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId4"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
     </sheetView>
@@ -8601,28 +8644,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+      <c r="A1" s="6" t="s">
         <v>578</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>770</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>771</v>
+      <c r="B1" s="6" t="s">
+        <v>768</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>769</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14"/>
-      <c r="B2" s="7"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="6"/>
       <c r="C2" s="3" t="s">
-        <v>802</v>
+        <v>799</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="7"/>
+      <c r="A3" s="13"/>
+      <c r="B3" s="6"/>
       <c r="C3" s="3" t="s">
-        <v>809</v>
+        <v>806</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
@@ -8645,143 +8688,143 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>789</v>
+        <v>786</v>
       </c>
       <c r="B6" s="2"/>
-      <c r="C6" s="18" t="s">
-        <v>790</v>
+      <c r="C6" s="14" t="s">
+        <v>787</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>734</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>735</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>736</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>736</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>737</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>738</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>739</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>738</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>740</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>741</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>742</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="135" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>742</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>743</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>744</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>745</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>745</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>746</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>747</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>748</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
+        <v>747</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>748</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>749</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>750</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>751</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
+        <v>750</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>751</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>752</v>
-      </c>
-      <c r="B13" s="3" t="s">
-        <v>753</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>754</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>753</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>754</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>755</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>756</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>757</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
+        <v>756</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>757</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>758</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>759</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>760</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="255" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>759</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>760</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>761</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>762</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>763</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>762</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>763</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>764</v>
-      </c>
-      <c r="B17" s="3" t="s">
-        <v>765</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>766</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
+        <v>765</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>766</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>767</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>768</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>769</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update new notation for methods
</commit_message>
<xml_diff>
--- a/geochemistry/AnalyticalMethodNotation.xlsx
+++ b/geochemistry/AnalyticalMethodNotation.xlsx
@@ -8,10 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944a82e2ddcde9eb/Documents/GithubC/Astromat/Vocabulary/geochemistry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="116" documentId="13_ncr:40009_{DC6A8E47-B5AA-4822-9869-B2DEB139BBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{58DCD148-F566-4C2C-95E8-F6AAAAA2BA1D}"/>
+  <xr:revisionPtr revIDLastSave="270" documentId="13_ncr:40009_{DC6A8E47-B5AA-4822-9869-B2DEB139BBC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1F7449B7-855B-4F78-BBC4-43690BE46B7F}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21585" windowHeight="12645" xr2:uid="{91CF9590-0788-40CF-A57F-B8740DE6F464}"/>
+    <workbookView xWindow="315" yWindow="2220" windowWidth="17550" windowHeight="13905" xr2:uid="{91CF9590-0788-40CF-A57F-B8740DE6F464}"/>
   </bookViews>
   <sheets>
     <sheet name="AnalyticalMethodNotation" sheetId="1" r:id="rId1"/>
@@ -19,7 +18,7 @@
     <sheet name="explanation of sources" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AnalyticalMethodNotation!$F$1:$F$248</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">AnalyticalMethodNotation!$B$1:$B$248</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -73,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1653" uniqueCount="841">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1652" uniqueCount="847">
   <si>
     <t>notation</t>
   </si>
@@ -2942,12 +2941,30 @@
 https://en.wikipedia.org/wiki/Cavity_ring-down_spectroscopy
 https://gcmd.earthdata.nasa.gov/KeywordViewer/scheme/all/9a61fcbd-c75f-4940-939f-6e4c7d84d643</t>
   </si>
+  <si>
+    <t>EEL-S</t>
+  </si>
+  <si>
+    <t>EA-IR-S</t>
+  </si>
+  <si>
+    <t>CE-A-S</t>
+  </si>
+  <si>
+    <t>CRD-S</t>
+  </si>
+  <si>
+    <t>ED-XF-S</t>
+  </si>
+  <si>
+    <t>ICP-SF-MS</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="25" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3122,16 +3139,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="38">
+  <fills count="37">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3335,12 +3344,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -3503,7 +3506,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3560,19 +3563,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" quotePrefix="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6" quotePrefix="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -3636,10 +3636,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3961,12 +3957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G248"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A189" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C185" sqref="C185"/>
-    </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="1">
-      <selection activeCell="C30" sqref="C30:C31"/>
+    <sheetView tabSelected="1" topLeftCell="B35" workbookViewId="0">
+      <selection activeCell="D228" sqref="C228:D228"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4022,7 +4014,7 @@
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="23" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
@@ -4037,11 +4029,11 @@
       </c>
       <c r="G3" s="2"/>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="23" t="s">
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -4132,7 +4124,7 @@
       <c r="A9" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="23" t="s">
         <v>25</v>
       </c>
       <c r="C9" s="2" t="s">
@@ -4166,7 +4158,7 @@
     </row>
     <row r="11" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="23" t="s">
         <v>30</v>
       </c>
       <c r="C11" s="2" t="s">
@@ -4256,7 +4248,7 @@
       <c r="A16" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="23" t="s">
         <v>40</v>
       </c>
       <c r="C16" s="2" t="s">
@@ -4271,9 +4263,9 @@
       </c>
       <c r="G16" s="2"/>
     </row>
-    <row r="17" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="23" t="s">
         <v>21</v>
       </c>
       <c r="C17" s="2" t="s">
@@ -4311,7 +4303,7 @@
       <c r="A19" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="23" t="s">
         <v>46</v>
       </c>
       <c r="C19" s="2" t="s">
@@ -4400,7 +4392,7 @@
       <c r="A24" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="23" t="s">
         <v>54</v>
       </c>
       <c r="C24" s="2" t="s">
@@ -4470,7 +4462,7 @@
       <c r="A28" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="23" t="s">
         <v>66</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -4489,7 +4481,7 @@
       <c r="A29" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="23" t="s">
         <v>70</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -4506,13 +4498,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="17"/>
-      <c r="B30" s="17" t="s">
-        <v>837</v>
+      <c r="B30" s="23" t="s">
+        <v>843</v>
       </c>
       <c r="C30" s="17" t="s">
         <v>835</v>
       </c>
-      <c r="D30" s="24" t="s">
+      <c r="D30" s="21" t="s">
         <v>836</v>
       </c>
       <c r="E30" s="18"/>
@@ -4523,13 +4515,13 @@
     </row>
     <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="17"/>
-      <c r="B31" s="17" t="s">
-        <v>839</v>
+      <c r="B31" s="23" t="s">
+        <v>844</v>
       </c>
       <c r="C31" s="17" t="s">
         <v>838</v>
       </c>
-      <c r="D31" s="25" t="s">
+      <c r="D31" s="22" t="s">
         <v>840</v>
       </c>
       <c r="E31" s="18"/>
@@ -4559,7 +4551,7 @@
       <c r="A33" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="23" t="s">
         <v>76</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -4610,7 +4602,7 @@
     </row>
     <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
-      <c r="B36" s="17" t="s">
+      <c r="B36" s="23" t="s">
         <v>816</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -4630,7 +4622,7 @@
       <c r="A37" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="23" t="s">
         <v>81</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -4649,7 +4641,7 @@
       <c r="A38" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="23" t="s">
         <v>89</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -4700,7 +4692,7 @@
     </row>
     <row r="41" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="23" t="s">
         <v>773</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -4721,7 +4713,7 @@
       <c r="A42" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="B42" s="2" t="s">
+      <c r="B42" s="23" t="s">
         <v>91</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -4757,7 +4749,7 @@
       <c r="A44" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="23" t="s">
         <v>102</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -4825,7 +4817,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="12"/>
-      <c r="B48" s="2" t="s">
+      <c r="B48" s="23" t="s">
         <v>805</v>
       </c>
       <c r="C48" s="2" t="s">
@@ -4847,7 +4839,7 @@
       <c r="A49" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="23" t="s">
         <v>110</v>
       </c>
       <c r="C49" s="2" t="s">
@@ -4868,7 +4860,7 @@
       <c r="A50" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="23" t="s">
         <v>116</v>
       </c>
       <c r="C50" s="2" t="s">
@@ -4902,7 +4894,7 @@
     </row>
     <row r="52" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A52" s="12"/>
-      <c r="B52" s="17" t="s">
+      <c r="B52" s="23" t="s">
         <v>817</v>
       </c>
       <c r="C52" s="2" t="s">
@@ -4922,7 +4914,7 @@
       <c r="A53" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="23" t="s">
         <v>122</v>
       </c>
       <c r="C53" s="2" t="s">
@@ -4939,7 +4931,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="12"/>
-      <c r="B54" s="17" t="s">
+      <c r="B54" s="23" t="s">
         <v>820</v>
       </c>
       <c r="C54" s="2" t="s">
@@ -4961,7 +4953,7 @@
       <c r="A55" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="23" t="s">
         <v>126</v>
       </c>
       <c r="C55" s="2" t="s">
@@ -4980,7 +4972,7 @@
       <c r="A56" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="23" t="s">
         <v>130</v>
       </c>
       <c r="C56" s="2" t="s">
@@ -5014,7 +5006,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
-      <c r="B58" s="17" t="s">
+      <c r="B58" s="23" t="s">
         <v>818</v>
       </c>
       <c r="C58" s="2" t="s">
@@ -5032,8 +5024,8 @@
     </row>
     <row r="59" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
-      <c r="B59" s="2" t="s">
-        <v>774</v>
+      <c r="B59" s="23" t="s">
+        <v>841</v>
       </c>
       <c r="C59" s="2" t="s">
         <v>136</v>
@@ -5053,7 +5045,7 @@
       <c r="A60" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="23" t="s">
         <v>138</v>
       </c>
       <c r="C60" s="2" t="s">
@@ -5089,7 +5081,7 @@
       <c r="A62" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="23" t="s">
         <v>145</v>
       </c>
       <c r="C62" s="2" t="s">
@@ -5127,7 +5119,7 @@
       <c r="A64" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="23" t="s">
         <v>152</v>
       </c>
       <c r="C64" s="2" t="s">
@@ -5163,8 +5155,8 @@
     </row>
     <row r="66" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A66" s="12"/>
-      <c r="B66" s="2" t="s">
-        <v>807</v>
+      <c r="B66" s="23" t="s">
+        <v>842</v>
       </c>
       <c r="C66" s="2" t="s">
         <v>157</v>
@@ -5177,7 +5169,7 @@
       </c>
       <c r="F66" s="2" t="str">
         <f>B66</f>
-        <v>EA-IR</v>
+        <v>EA-IR-S</v>
       </c>
       <c r="G66" s="2"/>
     </row>
@@ -5185,7 +5177,7 @@
       <c r="A67" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="23" t="s">
         <v>159</v>
       </c>
       <c r="C67" s="2" t="s">
@@ -5204,7 +5196,7 @@
       <c r="A68" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="23" t="s">
         <v>163</v>
       </c>
       <c r="C68" s="2" t="s">
@@ -5223,7 +5215,7 @@
       <c r="A69" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="23" t="s">
         <v>166</v>
       </c>
       <c r="C69" s="2" t="s">
@@ -5242,7 +5234,7 @@
       <c r="A70" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B70" s="2" t="s">
+      <c r="B70" s="23" t="s">
         <v>169</v>
       </c>
       <c r="C70" s="2" t="s">
@@ -5261,8 +5253,8 @@
       <c r="A71" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="B71" s="2" t="s">
-        <v>172</v>
+      <c r="B71" s="23" t="s">
+        <v>845</v>
       </c>
       <c r="C71" s="2" t="s">
         <v>173</v>
@@ -5278,7 +5270,7 @@
     </row>
     <row r="72" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="23" t="s">
         <v>777</v>
       </c>
       <c r="C72" s="2" t="s">
@@ -5299,7 +5291,7 @@
       <c r="A73" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="23" t="s">
         <v>177</v>
       </c>
       <c r="C73" s="2" t="s">
@@ -5388,7 +5380,7 @@
       <c r="A78" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="23" t="s">
         <v>87</v>
       </c>
       <c r="C78" s="2" t="s">
@@ -5424,7 +5416,7 @@
       <c r="A80" s="2" t="s">
         <v>193</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B80" s="23" t="s">
         <v>194</v>
       </c>
       <c r="C80" s="2" t="s">
@@ -5441,7 +5433,7 @@
     </row>
     <row r="81" spans="1:7" ht="150" x14ac:dyDescent="0.25">
       <c r="A81" s="12"/>
-      <c r="B81" s="17" t="s">
+      <c r="B81" s="23" t="s">
         <v>821</v>
       </c>
       <c r="C81" s="2" t="s">
@@ -5461,7 +5453,7 @@
     </row>
     <row r="82" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A82" s="12"/>
-      <c r="B82" s="17" t="s">
+      <c r="B82" s="23" t="s">
         <v>819</v>
       </c>
       <c r="C82" s="2" t="s">
@@ -5483,7 +5475,7 @@
       <c r="A83" s="2" t="s">
         <v>199</v>
       </c>
-      <c r="B83" s="2" t="s">
+      <c r="B83" s="23" t="s">
         <v>200</v>
       </c>
       <c r="C83" s="2" t="s">
@@ -5536,7 +5528,7 @@
       <c r="A86" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="B86" s="2" t="s">
+      <c r="B86" s="23" t="s">
         <v>207</v>
       </c>
       <c r="C86" s="2" t="s">
@@ -5572,7 +5564,7 @@
       <c r="A88" s="2" t="s">
         <v>210</v>
       </c>
-      <c r="B88" s="2" t="s">
+      <c r="B88" s="23" t="s">
         <v>211</v>
       </c>
       <c r="C88" s="2" t="s">
@@ -5593,7 +5585,7 @@
       <c r="A89" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="B89" s="2" t="s">
+      <c r="B89" s="23" t="s">
         <v>214</v>
       </c>
       <c r="C89" s="2" t="s">
@@ -5717,7 +5709,7 @@
       <c r="A96" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="B96" s="2" t="s">
+      <c r="B96" s="23" t="s">
         <v>128</v>
       </c>
       <c r="C96" s="2" t="s">
@@ -5784,13 +5776,13 @@
       <c r="G99" s="2"/>
     </row>
     <row r="100" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A100" s="2" t="s">
+      <c r="A100" s="23" t="s">
         <v>236</v>
       </c>
-      <c r="B100" s="2" t="s">
+      <c r="B100" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="C100" s="2" t="s">
+      <c r="C100" s="23" t="s">
         <v>582</v>
       </c>
       <c r="D100" s="3" t="s">
@@ -5804,7 +5796,7 @@
     </row>
     <row r="101" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A101" s="12"/>
-      <c r="B101" s="17" t="s">
+      <c r="B101" s="23" t="s">
         <v>823</v>
       </c>
       <c r="C101" s="2" t="s">
@@ -5859,7 +5851,7 @@
       <c r="A104" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="B104" s="2" t="s">
+      <c r="B104" s="23" t="s">
         <v>242</v>
       </c>
       <c r="C104" s="2" t="s">
@@ -5878,7 +5870,7 @@
       <c r="A105" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="B105" s="2" t="s">
+      <c r="B105" s="23" t="s">
         <v>245</v>
       </c>
       <c r="C105" s="2" t="s">
@@ -5897,7 +5889,7 @@
       <c r="A106" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="B106" s="2" t="s">
+      <c r="B106" s="23" t="s">
         <v>248</v>
       </c>
       <c r="C106" s="2" t="s">
@@ -5916,7 +5908,7 @@
       <c r="A107" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B107" s="2" t="s">
+      <c r="B107" s="23" t="s">
         <v>251</v>
       </c>
       <c r="C107" s="2" t="s">
@@ -5932,11 +5924,11 @@
       <c r="G107" s="2"/>
     </row>
     <row r="108" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A108" s="7"/>
+      <c r="A108" s="23"/>
       <c r="B108" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="C108" s="21" t="s">
+      <c r="C108" s="23" t="s">
         <v>254</v>
       </c>
       <c r="D108" s="3" t="s">
@@ -5989,7 +5981,7 @@
       <c r="A111" s="2" t="s">
         <v>260</v>
       </c>
-      <c r="B111" s="2" t="s">
+      <c r="B111" s="23" t="s">
         <v>261</v>
       </c>
       <c r="C111" s="2" t="s">
@@ -6008,7 +6000,7 @@
       <c r="A112" s="2" t="s">
         <v>263</v>
       </c>
-      <c r="B112" s="2" t="s">
+      <c r="B112" s="23" t="s">
         <v>264</v>
       </c>
       <c r="C112" s="2" t="s">
@@ -6078,7 +6070,7 @@
       <c r="A116" s="2" t="s">
         <v>272</v>
       </c>
-      <c r="B116" s="2" t="s">
+      <c r="B116" s="23" t="s">
         <v>273</v>
       </c>
       <c r="C116" s="2" t="s">
@@ -6097,7 +6089,7 @@
       <c r="A117" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="B117" s="2" t="s">
+      <c r="B117" s="23" t="s">
         <v>276</v>
       </c>
       <c r="C117" s="2" t="s">
@@ -6116,7 +6108,7 @@
       <c r="A118" s="2" t="s">
         <v>279</v>
       </c>
-      <c r="B118" s="2" t="s">
+      <c r="B118" s="23" t="s">
         <v>280</v>
       </c>
       <c r="C118" s="2" t="s">
@@ -6135,7 +6127,7 @@
       <c r="A119" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="B119" s="2" t="s">
+      <c r="B119" s="23" t="s">
         <v>283</v>
       </c>
       <c r="C119" s="2" t="s">
@@ -6154,7 +6146,7 @@
       <c r="A120" s="2" t="s">
         <v>286</v>
       </c>
-      <c r="B120" s="2" t="s">
+      <c r="B120" s="23" t="s">
         <v>287</v>
       </c>
       <c r="C120" s="2" t="s">
@@ -6173,7 +6165,7 @@
       <c r="A121" s="2" t="s">
         <v>289</v>
       </c>
-      <c r="B121" s="2" t="s">
+      <c r="B121" s="23" t="s">
         <v>290</v>
       </c>
       <c r="C121" s="2" t="s">
@@ -6192,7 +6184,7 @@
       <c r="A122" s="2" t="s">
         <v>292</v>
       </c>
-      <c r="B122" s="2" t="s">
+      <c r="B122" s="23" t="s">
         <v>293</v>
       </c>
       <c r="C122" s="2" t="s">
@@ -6211,7 +6203,7 @@
       <c r="A123" s="2" t="s">
         <v>295</v>
       </c>
-      <c r="B123" s="2" t="s">
+      <c r="B123" s="23" t="s">
         <v>296</v>
       </c>
       <c r="C123" s="2" t="s">
@@ -6230,7 +6222,7 @@
       <c r="A124" s="2" t="s">
         <v>298</v>
       </c>
-      <c r="B124" s="2" t="s">
+      <c r="B124" s="23" t="s">
         <v>299</v>
       </c>
       <c r="C124" s="2" t="s">
@@ -6266,7 +6258,7 @@
       <c r="A126" s="2" t="s">
         <v>303</v>
       </c>
-      <c r="B126" s="2" t="s">
+      <c r="B126" s="23" t="s">
         <v>304</v>
       </c>
       <c r="C126" s="2" t="s">
@@ -6319,7 +6311,7 @@
       <c r="A129" s="2" t="s">
         <v>310</v>
       </c>
-      <c r="B129" s="2" t="s">
+      <c r="B129" s="23" t="s">
         <v>311</v>
       </c>
       <c r="C129" s="2" t="s">
@@ -6336,7 +6328,7 @@
     </row>
     <row r="130" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
-      <c r="B130" s="2" t="s">
+      <c r="B130" s="23" t="s">
         <v>779</v>
       </c>
       <c r="C130" s="2" t="s">
@@ -6372,7 +6364,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="12"/>
-      <c r="B132" s="20" t="s">
+      <c r="B132" s="24" t="s">
         <v>831</v>
       </c>
       <c r="C132" s="2" t="s">
@@ -6411,9 +6403,7 @@
       <c r="A134" s="2" t="s">
         <v>319</v>
       </c>
-      <c r="B134" s="2" t="s">
-        <v>319</v>
-      </c>
+      <c r="B134" s="2"/>
       <c r="C134" s="2" t="s">
         <v>320</v>
       </c>
@@ -6430,7 +6420,7 @@
       <c r="A135" s="2" t="s">
         <v>321</v>
       </c>
-      <c r="B135" s="2" t="s">
+      <c r="B135" s="23" t="s">
         <v>322</v>
       </c>
       <c r="C135" s="2" t="s">
@@ -6449,7 +6439,7 @@
       <c r="A136" s="2" t="s">
         <v>325</v>
       </c>
-      <c r="B136" s="2" t="s">
+      <c r="B136" s="23" t="s">
         <v>326</v>
       </c>
       <c r="C136" s="2" t="s">
@@ -6468,7 +6458,7 @@
       <c r="A137" s="2" t="s">
         <v>328</v>
       </c>
-      <c r="B137" s="2" t="s">
+      <c r="B137" s="23" t="s">
         <v>190</v>
       </c>
       <c r="C137" s="2" t="s">
@@ -6558,7 +6548,7 @@
       <c r="A142" s="2" t="s">
         <v>340</v>
       </c>
-      <c r="B142" s="2" t="s">
+      <c r="B142" s="23" t="s">
         <v>341</v>
       </c>
       <c r="C142" s="2" t="s">
@@ -6577,7 +6567,7 @@
       <c r="A143" s="2" t="s">
         <v>343</v>
       </c>
-      <c r="B143" s="2" t="s">
+      <c r="B143" s="23" t="s">
         <v>257</v>
       </c>
       <c r="C143" s="2" t="s">
@@ -6598,7 +6588,7 @@
       <c r="A144" s="2" t="s">
         <v>346</v>
       </c>
-      <c r="B144" s="2" t="s">
+      <c r="B144" s="23" t="s">
         <v>347</v>
       </c>
       <c r="C144" s="2" t="s">
@@ -6619,7 +6609,7 @@
       <c r="A145" s="2" t="s">
         <v>349</v>
       </c>
-      <c r="B145" s="2" t="s">
+      <c r="B145" s="23" t="s">
         <v>350</v>
       </c>
       <c r="C145" s="2" t="s">
@@ -6638,7 +6628,7 @@
       <c r="A146" s="2" t="s">
         <v>353</v>
       </c>
-      <c r="B146" s="2" t="s">
+      <c r="B146" s="23" t="s">
         <v>354</v>
       </c>
       <c r="C146" s="2" t="s">
@@ -6691,7 +6681,7 @@
       <c r="A149" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="B149" s="2" t="s">
+      <c r="B149" s="23" t="s">
         <v>361</v>
       </c>
       <c r="C149" s="2" t="s">
@@ -6727,7 +6717,7 @@
       <c r="A151" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="B151" s="2" t="s">
+      <c r="B151" s="23" t="s">
         <v>366</v>
       </c>
       <c r="C151" s="2" t="s">
@@ -6746,7 +6736,7 @@
       <c r="A152" s="2" t="s">
         <v>368</v>
       </c>
-      <c r="B152" s="2" t="s">
+      <c r="B152" s="23" t="s">
         <v>369</v>
       </c>
       <c r="C152" s="2" t="s">
@@ -6799,7 +6789,7 @@
       <c r="A155" s="2" t="s">
         <v>374</v>
       </c>
-      <c r="B155" s="2" t="s">
+      <c r="B155" s="23" t="s">
         <v>375</v>
       </c>
       <c r="C155" s="2" t="s">
@@ -6818,7 +6808,7 @@
       <c r="A156" s="2" t="s">
         <v>377</v>
       </c>
-      <c r="B156" s="2" t="s">
+      <c r="B156" s="23" t="s">
         <v>378</v>
       </c>
       <c r="C156" s="2" t="s">
@@ -6837,7 +6827,7 @@
       <c r="A157" s="2" t="s">
         <v>380</v>
       </c>
-      <c r="B157" s="2" t="s">
+      <c r="B157" s="23" t="s">
         <v>381</v>
       </c>
       <c r="C157" s="2" t="s">
@@ -6854,7 +6844,7 @@
     </row>
     <row r="158" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A158" s="2"/>
-      <c r="B158" s="2" t="s">
+      <c r="B158" s="23" t="s">
         <v>782</v>
       </c>
       <c r="C158" s="2" t="s">
@@ -6892,7 +6882,7 @@
       <c r="A160" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="B160" s="2" t="s">
+      <c r="B160" s="23" t="s">
         <v>387</v>
       </c>
       <c r="C160" s="2" t="s">
@@ -6928,7 +6918,7 @@
       <c r="A162" s="2" t="s">
         <v>391</v>
       </c>
-      <c r="B162" s="2" t="s">
+      <c r="B162" s="23" t="s">
         <v>392</v>
       </c>
       <c r="C162" s="2" t="s">
@@ -6947,7 +6937,7 @@
       <c r="A163" s="2" t="s">
         <v>394</v>
       </c>
-      <c r="B163" s="2" t="s">
+      <c r="B163" s="23" t="s">
         <v>395</v>
       </c>
       <c r="C163" s="2" t="s">
@@ -6983,7 +6973,7 @@
       <c r="A165" s="2" t="s">
         <v>400</v>
       </c>
-      <c r="B165" s="2" t="s">
+      <c r="B165" s="23" t="s">
         <v>48</v>
       </c>
       <c r="C165" s="2" t="s">
@@ -7017,7 +7007,7 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="12"/>
-      <c r="B167" s="20" t="s">
+      <c r="B167" s="24" t="s">
         <v>833</v>
       </c>
       <c r="C167" s="2" t="s">
@@ -7073,7 +7063,7 @@
       <c r="A170" s="2" t="s">
         <v>409</v>
       </c>
-      <c r="B170" s="2" t="s">
+      <c r="B170" s="23" t="s">
         <v>410</v>
       </c>
       <c r="C170" s="2" t="s">
@@ -7110,7 +7100,7 @@
       <c r="A172" s="2" t="s">
         <v>414</v>
       </c>
-      <c r="B172" s="2" t="s">
+      <c r="B172" s="23" t="s">
         <v>415</v>
       </c>
       <c r="C172" s="2" t="s">
@@ -7129,7 +7119,7 @@
       <c r="A173" s="2" t="s">
         <v>417</v>
       </c>
-      <c r="B173" s="2" t="s">
+      <c r="B173" s="23" t="s">
         <v>418</v>
       </c>
       <c r="C173" s="2" t="s">
@@ -7148,7 +7138,7 @@
       <c r="A174" s="2" t="s">
         <v>420</v>
       </c>
-      <c r="B174" s="2" t="s">
+      <c r="B174" s="23" t="s">
         <v>421</v>
       </c>
       <c r="C174" s="2" t="s">
@@ -7169,7 +7159,7 @@
       <c r="A175" s="2" t="s">
         <v>425</v>
       </c>
-      <c r="B175" s="2" t="s">
+      <c r="B175" s="23" t="s">
         <v>426</v>
       </c>
       <c r="C175" s="2" t="s">
@@ -7188,7 +7178,7 @@
       <c r="A176" s="2" t="s">
         <v>392</v>
       </c>
-      <c r="B176" s="2" t="s">
+      <c r="B176" s="23" t="s">
         <v>428</v>
       </c>
       <c r="C176" s="2" t="s">
@@ -7224,7 +7214,7 @@
     </row>
     <row r="178" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A178" s="12"/>
-      <c r="B178" s="17" t="s">
+      <c r="B178" s="23" t="s">
         <v>825</v>
       </c>
       <c r="C178" s="2" t="s">
@@ -7246,7 +7236,7 @@
       <c r="A179" s="2" t="s">
         <v>434</v>
       </c>
-      <c r="B179" s="2" t="s">
+      <c r="B179" s="23" t="s">
         <v>435</v>
       </c>
       <c r="C179" s="2" t="s">
@@ -7280,7 +7270,7 @@
     </row>
     <row r="181" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A181" s="12"/>
-      <c r="B181" s="2" t="s">
+      <c r="B181" s="23" t="s">
         <v>809</v>
       </c>
       <c r="C181" s="2" t="s">
@@ -7319,7 +7309,7 @@
       <c r="A183" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="B183" s="2" t="s">
+      <c r="B183" s="23" t="s">
         <v>339</v>
       </c>
       <c r="C183" s="2" t="s">
@@ -7338,7 +7328,7 @@
       <c r="A184" s="2" t="s">
         <v>443</v>
       </c>
-      <c r="B184" s="2" t="s">
+      <c r="B184" s="23" t="s">
         <v>313</v>
       </c>
       <c r="C184" s="2" t="s">
@@ -7357,7 +7347,7 @@
       <c r="A185" s="2" t="s">
         <v>445</v>
       </c>
-      <c r="B185" s="2" t="s">
+      <c r="B185" s="23" t="s">
         <v>446</v>
       </c>
       <c r="C185" s="2" t="s">
@@ -7376,7 +7366,7 @@
       <c r="A186" s="2" t="s">
         <v>448</v>
       </c>
-      <c r="B186" s="2" t="s">
+      <c r="B186" s="23" t="s">
         <v>285</v>
       </c>
       <c r="C186" s="2" t="s">
@@ -7395,7 +7385,7 @@
       <c r="A187" s="2" t="s">
         <v>450</v>
       </c>
-      <c r="B187" s="2" t="s">
+      <c r="B187" s="23" t="s">
         <v>451</v>
       </c>
       <c r="C187" s="2" t="s">
@@ -7416,7 +7406,7 @@
       <c r="A188" s="2" t="s">
         <v>454</v>
       </c>
-      <c r="B188" s="2" t="s">
+      <c r="B188" s="23" t="s">
         <v>455</v>
       </c>
       <c r="C188" s="2" t="s">
@@ -7437,7 +7427,7 @@
       <c r="A189" s="2" t="s">
         <v>458</v>
       </c>
-      <c r="B189" s="2" t="s">
+      <c r="B189" s="23" t="s">
         <v>459</v>
       </c>
       <c r="C189" s="2" t="s">
@@ -7490,7 +7480,7 @@
       <c r="A192" s="2" t="s">
         <v>466</v>
       </c>
-      <c r="B192" s="2" t="s">
+      <c r="B192" s="23" t="s">
         <v>467</v>
       </c>
       <c r="C192" s="2" t="s">
@@ -7507,7 +7497,7 @@
     </row>
     <row r="193" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A193" s="12"/>
-      <c r="B193" s="17" t="s">
+      <c r="B193" s="23" t="s">
         <v>826</v>
       </c>
       <c r="C193" s="2" t="s">
@@ -7525,7 +7515,7 @@
     </row>
     <row r="194" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A194" s="2"/>
-      <c r="B194" s="2" t="s">
+      <c r="B194" s="23" t="s">
         <v>786</v>
       </c>
       <c r="C194" s="2" t="s">
@@ -7546,7 +7536,7 @@
       <c r="A195" s="2" t="s">
         <v>471</v>
       </c>
-      <c r="B195" s="2" t="s">
+      <c r="B195" s="23" t="s">
         <v>472</v>
       </c>
       <c r="C195" s="2" t="s">
@@ -7563,7 +7553,7 @@
     </row>
     <row r="196" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A196" s="12"/>
-      <c r="B196" s="17" t="s">
+      <c r="B196" s="23" t="s">
         <v>822</v>
       </c>
       <c r="C196" s="2" t="s">
@@ -7617,7 +7607,7 @@
       <c r="A199" s="2" t="s">
         <v>478</v>
       </c>
-      <c r="B199" s="2" t="s">
+      <c r="B199" s="23" t="s">
         <v>479</v>
       </c>
       <c r="C199" s="2" t="s">
@@ -7636,7 +7626,7 @@
       <c r="A200" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="B200" s="2" t="s">
+      <c r="B200" s="23" t="s">
         <v>482</v>
       </c>
       <c r="C200" s="2" t="s">
@@ -7655,8 +7645,8 @@
       <c r="A201" s="2" t="s">
         <v>484</v>
       </c>
-      <c r="B201" s="2" t="s">
-        <v>485</v>
+      <c r="B201" s="23" t="s">
+        <v>846</v>
       </c>
       <c r="C201" s="2" t="s">
         <v>486</v>
@@ -7674,7 +7664,7 @@
       <c r="A202" s="2" t="s">
         <v>487</v>
       </c>
-      <c r="B202" s="2" t="s">
+      <c r="B202" s="23" t="s">
         <v>488</v>
       </c>
       <c r="C202" s="2" t="s">
@@ -7710,7 +7700,7 @@
     </row>
     <row r="204" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A204" s="12"/>
-      <c r="B204" s="17" t="s">
+      <c r="B204" s="23" t="s">
         <v>827</v>
       </c>
       <c r="C204" s="2" t="s">
@@ -7728,7 +7718,7 @@
     </row>
     <row r="205" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A205" s="12"/>
-      <c r="B205" s="17" t="s">
+      <c r="B205" s="23" t="s">
         <v>828</v>
       </c>
       <c r="C205" s="2" t="s">
@@ -7748,7 +7738,7 @@
       <c r="A206" s="2" t="s">
         <v>495</v>
       </c>
-      <c r="B206" s="2" t="s">
+      <c r="B206" s="23" t="s">
         <v>496</v>
       </c>
       <c r="C206" s="2" t="s">
@@ -7767,7 +7757,7 @@
       <c r="A207" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="B207" s="2" t="s">
+      <c r="B207" s="23" t="s">
         <v>499</v>
       </c>
       <c r="C207" s="2" t="s">
@@ -7788,7 +7778,7 @@
       <c r="A208" s="2" t="s">
         <v>502</v>
       </c>
-      <c r="B208" s="2" t="s">
+      <c r="B208" s="23" t="s">
         <v>503</v>
       </c>
       <c r="C208" s="2" t="s">
@@ -7809,7 +7799,7 @@
       <c r="A209" s="2" t="s">
         <v>507</v>
       </c>
-      <c r="B209" s="2" t="s">
+      <c r="B209" s="23" t="s">
         <v>508</v>
       </c>
       <c r="C209" s="2" t="s">
@@ -7828,7 +7818,7 @@
       <c r="A210" s="2" t="s">
         <v>510</v>
       </c>
-      <c r="B210" s="2" t="s">
+      <c r="B210" s="23" t="s">
         <v>511</v>
       </c>
       <c r="C210" s="2" t="s">
@@ -7898,7 +7888,7 @@
       <c r="A214" s="2" t="s">
         <v>518</v>
       </c>
-      <c r="B214" s="2" t="s">
+      <c r="B214" s="23" t="s">
         <v>519</v>
       </c>
       <c r="C214" s="2" t="s">
@@ -7917,7 +7907,7 @@
       <c r="A215" s="2" t="s">
         <v>522</v>
       </c>
-      <c r="B215" s="2" t="s">
+      <c r="B215" s="23" t="s">
         <v>523</v>
       </c>
       <c r="C215" s="2" t="s">
@@ -7936,7 +7926,7 @@
       <c r="A216" s="2" t="s">
         <v>525</v>
       </c>
-      <c r="B216" s="2" t="s">
+      <c r="B216" s="23" t="s">
         <v>58</v>
       </c>
       <c r="C216" s="2" t="s">
@@ -7970,7 +7960,7 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="12"/>
-      <c r="B218" s="17" t="s">
+      <c r="B218" s="23" t="s">
         <v>829</v>
       </c>
       <c r="C218" s="2" t="s">
@@ -7992,7 +7982,7 @@
       <c r="A219" s="2" t="s">
         <v>529</v>
       </c>
-      <c r="B219" s="2" t="s">
+      <c r="B219" s="23" t="s">
         <v>530</v>
       </c>
       <c r="C219" s="2" t="s">
@@ -8011,7 +8001,7 @@
       <c r="A220" s="2" t="s">
         <v>532</v>
       </c>
-      <c r="B220" s="2" t="s">
+      <c r="B220" s="23" t="s">
         <v>533</v>
       </c>
       <c r="C220" s="2" t="s">
@@ -8028,7 +8018,7 @@
     </row>
     <row r="221" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A221" s="2"/>
-      <c r="B221" s="2" t="s">
+      <c r="B221" s="23" t="s">
         <v>789</v>
       </c>
       <c r="C221" s="2" t="s">
@@ -8064,7 +8054,7 @@
     </row>
     <row r="223" spans="1:7" ht="165" x14ac:dyDescent="0.25">
       <c r="A223" s="2"/>
-      <c r="B223" s="2" t="s">
+      <c r="B223" s="23" t="s">
         <v>791</v>
       </c>
       <c r="C223" s="2" t="s">
@@ -8083,7 +8073,7 @@
     </row>
     <row r="224" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A224" s="2"/>
-      <c r="B224" s="2" t="s">
+      <c r="B224" s="23" t="s">
         <v>792</v>
       </c>
       <c r="C224" s="2" t="s">
@@ -8119,7 +8109,7 @@
       <c r="A226" s="2" t="s">
         <v>541</v>
       </c>
-      <c r="B226" s="2" t="s">
+      <c r="B226" s="23" t="s">
         <v>324</v>
       </c>
       <c r="C226" s="2" t="s">
@@ -8138,7 +8128,7 @@
       <c r="A227" s="2" t="s">
         <v>543</v>
       </c>
-      <c r="B227" s="2" t="s">
+      <c r="B227" s="23" t="s">
         <v>544</v>
       </c>
       <c r="C227" s="2" t="s">
@@ -8174,7 +8164,7 @@
       <c r="A229" s="2" t="s">
         <v>548</v>
       </c>
-      <c r="B229" s="2" t="s">
+      <c r="B229" s="23" t="s">
         <v>352</v>
       </c>
       <c r="C229" s="2" t="s">
@@ -8191,7 +8181,7 @@
     </row>
     <row r="230" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A230" s="2"/>
-      <c r="B230" s="2" t="s">
+      <c r="B230" s="23" t="s">
         <v>795</v>
       </c>
       <c r="C230" s="2" t="s">
@@ -8212,7 +8202,7 @@
       <c r="A231" s="2" t="s">
         <v>552</v>
       </c>
-      <c r="B231" s="2" t="s">
+      <c r="B231" s="23" t="s">
         <v>461</v>
       </c>
       <c r="C231" s="2" t="s">
@@ -8282,7 +8272,7 @@
       <c r="A235" s="2" t="s">
         <v>557</v>
       </c>
-      <c r="B235" s="2" t="s">
+      <c r="B235" s="23" t="s">
         <v>196</v>
       </c>
       <c r="C235" s="2" t="s">
@@ -8299,7 +8289,7 @@
     </row>
     <row r="236" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A236" s="2"/>
-      <c r="B236" s="2" t="s">
+      <c r="B236" s="23" t="s">
         <v>799</v>
       </c>
       <c r="C236" s="2" t="s">
@@ -8337,7 +8327,7 @@
       <c r="A238" s="2" t="s">
         <v>561</v>
       </c>
-      <c r="B238" s="2" t="s">
+      <c r="B238" s="23" t="s">
         <v>140</v>
       </c>
       <c r="C238" s="2" t="s">
@@ -8356,7 +8346,7 @@
       <c r="A239" s="2" t="s">
         <v>563</v>
       </c>
-      <c r="B239" s="2" t="s">
+      <c r="B239" s="23" t="s">
         <v>148</v>
       </c>
       <c r="C239" s="2" t="s">
@@ -8477,7 +8467,7 @@
     </row>
     <row r="246" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A246" s="2"/>
-      <c r="B246" s="2" t="s">
+      <c r="B246" s="23" t="s">
         <v>802</v>
       </c>
       <c r="C246" s="2" t="s">
@@ -8515,7 +8505,7 @@
       <c r="A248" s="2" t="s">
         <v>574</v>
       </c>
-      <c r="B248" s="2" t="s">
+      <c r="B248" s="23" t="s">
         <v>550</v>
       </c>
       <c r="C248" s="2" t="s">
@@ -8531,6 +8521,7 @@
       <c r="G248" s="2"/>
     </row>
   </sheetData>
+  <autoFilter ref="B1:B248" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F248">
     <sortCondition ref="C2:C248"/>
   </sortState>
@@ -8547,10 +8538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4CE2E11-1B68-4070-90EE-AFE307E2B226}">
   <dimension ref="A1:B246"/>
   <sheetViews>
-    <sheetView topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8629,7 +8617,7 @@
       <c r="A11" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="20" t="s">
         <v>21</v>
       </c>
     </row>
@@ -8637,7 +8625,7 @@
       <c r="A12" s="2" t="s">
         <v>834</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="20" t="s">
         <v>834</v>
       </c>
     </row>
@@ -10525,11 +10513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C8" sqref="C8"/>
-    </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>